<commit_message>
data driven update II
</commit_message>
<xml_diff>
--- a/test/e2e/resources/testData.xlsx
+++ b/test/e2e/resources/testData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shankerthebunker/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shankerthebunker/git/Protractor-Gradle/test/e2e/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{306DCF95-A917-3D4E-A713-933A60B21B3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F87DE4-B672-424D-BC1C-1D64A91A53CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{EEA41F1D-F66A-6940-9FA8-FD16FE9E2B92}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{EEA41F1D-F66A-6940-9FA8-FD16FE9E2B92}"/>
   </bookViews>
   <sheets>
     <sheet name="Add" sheetId="1" r:id="rId1"/>
@@ -29,19 +29,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
   <si>
     <t>_rowId</t>
   </si>
   <si>
-    <t>_DefaultCompRow</t>
+    <t>type@ValueOne</t>
+  </si>
+  <si>
+    <t>type@ValueTwo</t>
+  </si>
+  <si>
+    <t>verify@Output</t>
+  </si>
+  <si>
+    <t>Select@Operator</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>_DefaultCompRowOne</t>
+  </si>
+  <si>
+    <t>_DefaultCompRowTwo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -49,16 +79,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -66,12 +110,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,140 +446,400 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C65359-064E-204D-9E1E-9272B9F4A955}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{6DCDF7BD-FCAE-B640-AC51-F0167679AA7D}"/>
+    <hyperlink ref="D1" r:id="rId2" xr:uid="{0F435490-6FDA-A74A-8E49-C2B2A2444B7E}"/>
+    <hyperlink ref="E1" r:id="rId3" xr:uid="{D4AD9265-A032-3640-A87F-0FCA1CB2E957}"/>
+    <hyperlink ref="B1" r:id="rId4" xr:uid="{4302F1C3-D553-CD4B-97A2-C82B5DF24D28}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88FCECF9-8F9B-8C4A-9FB6-9AAF28DAD890}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{FF505370-5C0C-6D42-940F-DD10719AA86F}"/>
+    <hyperlink ref="D1" r:id="rId2" xr:uid="{E7E3DDB5-0EF2-A44F-AEDD-850BB85D9E3D}"/>
+    <hyperlink ref="E1" r:id="rId3" xr:uid="{3A1C6D8C-1E00-524A-A184-A68C75B472E4}"/>
+    <hyperlink ref="B1" r:id="rId4" xr:uid="{A4FA1A66-5103-9348-9789-1EBEA0669FFF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF60746-D662-6646-8535-6B3A645D5306}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{F0815FA4-A8B1-914B-83F4-EC3FE28ABEA4}"/>
+    <hyperlink ref="D1" r:id="rId2" xr:uid="{BE86AC07-E203-B44A-B8DD-AF0F0D8D8940}"/>
+    <hyperlink ref="E1" r:id="rId3" xr:uid="{0280C08C-DC21-2240-AC24-E2118F886741}"/>
+    <hyperlink ref="B1" r:id="rId4" xr:uid="{246A0A66-E8C8-F446-B615-6AA4C10BED98}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0D2FC6-B7BF-1B4A-AB03-D33116D7688F}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{5CFF414B-E6A6-824C-8C89-A02B1C6973F0}"/>
+    <hyperlink ref="D1" r:id="rId2" xr:uid="{6E19B40E-333A-8146-B07D-E2E9FA5BF31C}"/>
+    <hyperlink ref="E1" r:id="rId3" xr:uid="{57A94E06-0113-434E-B4F0-FC36F3CC1E7D}"/>
+    <hyperlink ref="B1" r:id="rId4" xr:uid="{546B72AC-214E-E245-9B1A-5530B1E94F44}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42773D75-1AE8-5B4F-8D92-EBF6451F4752}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{BFBC0060-C482-D941-B3EE-EA152BE27028}"/>
+    <hyperlink ref="D1" r:id="rId2" xr:uid="{E9B8463B-1B6C-B748-B680-3F7465D0D7B2}"/>
+    <hyperlink ref="E1" r:id="rId3" xr:uid="{0E2B77A5-0D57-9A40-B03D-AB918E63F7E2}"/>
+    <hyperlink ref="B1" r:id="rId4" xr:uid="{D3AFE72B-C990-8341-BAFD-880A104E2F1D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated for ApplitoolKit Dashboard
</commit_message>
<xml_diff>
--- a/test/e2e/resources/testData.xlsx
+++ b/test/e2e/resources/testData.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shankerthebunker/git/Protractor-Gradle/test/e2e/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C5A818-CDC1-EB47-91BC-BD3B68A8F932}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68292D47-5361-EC4C-AB0D-A7377C3D4AC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{EEA41F1D-F66A-6940-9FA8-FD16FE9E2B92}"/>
   </bookViews>
   <sheets>
-    <sheet name="Add" sheetId="1" r:id="rId1"/>
-    <sheet name="Substract" sheetId="2" r:id="rId2"/>
-    <sheet name="Divide" sheetId="3" r:id="rId3"/>
-    <sheet name="Multiply" sheetId="4" r:id="rId4"/>
-    <sheet name="Module" sheetId="5" r:id="rId5"/>
+    <sheet name="launchUrl" sheetId="6" r:id="rId1"/>
+    <sheet name="Add" sheetId="1" r:id="rId2"/>
+    <sheet name="Substract" sheetId="2" r:id="rId3"/>
+    <sheet name="Divide" sheetId="3" r:id="rId4"/>
+    <sheet name="Multiply" sheetId="4" r:id="rId5"/>
+    <sheet name="Module" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="15">
   <si>
     <t>_rowId</t>
   </si>
@@ -65,13 +66,22 @@
   </si>
   <si>
     <t>_DefaultCompRowTwo</t>
+  </si>
+  <si>
+    <t>Navigate@URL</t>
+  </si>
+  <si>
+    <t>_DefaultCompRow</t>
+  </si>
+  <si>
+    <t>http://juliemr.github.io/protractor-demo/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,6 +93,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,14 +144,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,12 +466,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A1BD46-8256-914C-A27D-4042979BBA53}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4C2D0F61-2F9E-7546-985A-F7377BEB77D5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C65359-064E-204D-9E1E-9272B9F4A955}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,7 +584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88FCECF9-8F9B-8C4A-9FB6-9AAF28DAD890}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -604,7 +664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF60746-D662-6646-8535-6B3A645D5306}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -684,7 +744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0D2FC6-B7BF-1B4A-AB03-D33116D7688F}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -764,7 +824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42773D75-1AE8-5B4F-8D92-EBF6451F4752}">
   <dimension ref="A1:E3"/>
   <sheetViews>

</xml_diff>